<commit_message>
fix model, init data
</commit_message>
<xml_diff>
--- a/RideSharing/Templates/BusStop_Export.xlsx
+++ b/RideSharing/Templates/BusStop_Export.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>[[Header]]</t>
   </si>
@@ -42,9 +42,6 @@
     <t>DeletedAt</t>
   </si>
   <si>
-    <t>Node</t>
-  </si>
-  <si>
     <t>DeliveryTrips</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
   </si>
   <si>
     <t>[[Data.DeletedAt]]</t>
-  </si>
-  <si>
-    <t>[[Data.Node.Name]]</t>
   </si>
   <si>
     <t>[[Data.DeliveryTrips]]</t>
@@ -489,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
@@ -529,7 +523,7 @@
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -545,28 +539,22 @@
       <c r="E6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="4" t="s">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>